<commit_message>
Add project scripts, documentation, and master data files
</commit_message>
<xml_diff>
--- a/Master/Master Input.xlsx
+++ b/Master/Master Input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Quotation\Master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C202679C-284D-42D4-A3A8-5BF9652CE90F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6979248-95D8-4AA8-9E25-7B77A8B30BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{19794FD9-2C50-4521-9D46-2A834FFCC96F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Quantity</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Yield loss %</t>
   </si>
   <si>
-    <t>Overhead Group (0-6)</t>
-  </si>
-  <si>
     <t>Freight </t>
   </si>
   <si>
@@ -104,9 +101,6 @@
     <t>Brand</t>
   </si>
   <si>
-    <t>Pack Size</t>
-  </si>
-  <si>
     <t>Other Cost</t>
   </si>
   <si>
@@ -120,6 +114,21 @@
   </si>
   <si>
     <t xml:space="preserve">RM Interest </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Group (0-6)</t>
+  </si>
+  <si>
+    <t>Pack Size 1</t>
+  </si>
+  <si>
+    <t>Pack Size2</t>
+  </si>
+  <si>
+    <t>Pack Size3</t>
+  </si>
+  <si>
+    <t>Product Code</t>
   </si>
 </sst>
 </file>
@@ -161,7 +170,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,6 +180,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -204,7 +243,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -213,14 +252,32 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -230,6 +287,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF66FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -558,142 +620,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4908C73C-C4DA-4B79-88E4-CF5830F4D48A}">
-  <dimension ref="A1:AB16"/>
+  <dimension ref="A1:AE16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AA2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.75" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" customWidth="1"/>
-    <col min="3" max="3" width="9.25" customWidth="1"/>
-    <col min="4" max="4" width="10.25" customWidth="1"/>
-    <col min="5" max="5" width="8.4140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.4140625" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" customWidth="1"/>
-    <col min="13" max="13" width="9.83203125" customWidth="1"/>
-    <col min="14" max="14" width="9.5" customWidth="1"/>
-    <col min="15" max="15" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.9140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.58203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.4140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="10.08203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.58203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.9140625" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11.08203125" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.9140625" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.4140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.4140625" customWidth="1"/>
+    <col min="13" max="15" width="10.6640625" customWidth="1"/>
+    <col min="16" max="16" width="9.83203125" customWidth="1"/>
+    <col min="17" max="17" width="9.5" customWidth="1"/>
+    <col min="18" max="18" width="15.1640625" customWidth="1"/>
+    <col min="19" max="19" width="9.83203125" customWidth="1"/>
+    <col min="20" max="20" width="17.33203125" customWidth="1"/>
+    <col min="21" max="21" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.4140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="27.08203125" customWidth="1"/>
+    <col min="26" max="26" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.08203125" customWidth="1"/>
+    <col min="29" max="29" width="13.08203125" customWidth="1"/>
+    <col min="30" max="30" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="8" customFormat="1" ht="33" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:31" s="7" customFormat="1" ht="33" x14ac:dyDescent="0.45">
+      <c r="A1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="7" t="s">
+      <c r="I1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="AC1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="V1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="X1" s="7" t="s">
+      <c r="AD1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="Y1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="AB1" s="7" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="1"/>
+      <c r="C2" s="2"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="3"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="5"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -707,18 +779,21 @@
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
-      <c r="X2" s="4"/>
+      <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="4"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="1"/>
+      <c r="C3" s="2"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -744,13 +819,16 @@
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
+      <c r="C4" s="2"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -776,13 +854,16 @@
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="1"/>
+      <c r="C5" s="2"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -808,13 +889,16 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
+      <c r="C6" s="2"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -840,13 +924,16 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="1"/>
+      <c r="C7" s="2"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -872,13 +959,16 @@
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="1"/>
+      <c r="C8" s="2"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -904,13 +994,16 @@
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="1"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -936,13 +1029,16 @@
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="1"/>
+      <c r="C10" s="2"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -968,13 +1064,16 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="1"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="1"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1000,13 +1099,16 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="1"/>
+      <c r="C12" s="2"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1032,13 +1134,16 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="1"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="1"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1064,13 +1169,16 @@
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="1"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="1"/>
+      <c r="C14" s="2"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1096,13 +1204,16 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="1"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="1"/>
+      <c r="C15" s="2"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1128,13 +1239,16 @@
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="1"/>
+      <c r="C16" s="2"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1160,6 +1274,9 @@
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.23622047244094491" right="0.15748031496062992" top="0.31496062992125984" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -1168,6 +1285,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cfdda32-5548-4012-ac44-2b82cbd5939e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="5fc4895e-a589-4c5e-b5d5-1fc939328557" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1176,7 +1304,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E3E9DF10A2D3054A81DA473217733159" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6ab41556a8e37d58bfcac66da3864cab">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8cfdda32-5548-4012-ac44-2b82cbd5939e" xmlns:ns3="5fc4895e-a589-4c5e-b5d5-1fc939328557" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fa5c69eb1ab36be3689b543fe7161763" ns2:_="" ns3:_="">
     <xsd:import namespace="8cfdda32-5548-4012-ac44-2b82cbd5939e"/>
@@ -1365,18 +1493,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cfdda32-5548-4012-ac44-2b82cbd5939e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="5fc4895e-a589-4c5e-b5d5-1fc939328557" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C33A24B-731B-486B-B89E-1EB2C2FEE187}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="5fc4895e-a589-4c5e-b5d5-1fc939328557"/>
+    <ds:schemaRef ds:uri="8cfdda32-5548-4012-ac44-2b82cbd5939e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{611BB65B-E243-4188-ADF7-2EBB63FCBC19}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1384,7 +1518,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99F0849F-BD3C-476E-B86C-9BCC38478A13}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1403,23 +1537,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C33A24B-731B-486B-B89E-1EB2C2FEE187}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="5fc4895e-a589-4c5e-b5d5-1fc939328557"/>
-    <ds:schemaRef ds:uri="8cfdda32-5548-4012-ac44-2b82cbd5939e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{58bb7255-ca8f-4031-9fe2-0e4ff45a2146}" enabled="0" method="" siteId="{58bb7255-ca8f-4031-9fe2-0e4ff45a2146}" removed="1"/>

</xml_diff>